<commit_message>
Se agrego una grafica en el excel
</commit_message>
<xml_diff>
--- a/numero_perfecto/pruebas.xlsx
+++ b/numero_perfecto/pruebas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Universidad\Analisis de Software\numero_perfecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC28\Documents\Analisis-Algoritmos\numero_perfecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF3D6A28-7E97-4E09-9759-9123FF54CFC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EDA5189-5A01-4FA3-8B15-D260C937EE27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{119C92B1-EED5-41A3-9A3B-CFA0F4C48975}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{119C92B1-EED5-41A3-9A3B-CFA0F4C48975}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>T1</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>win 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     </t>
   </si>
 </sst>
 </file>
@@ -149,10 +155,909 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$G$14:$G$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>34900</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>579220</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1770460</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1831360</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18653560</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18788020</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33067340</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80661940</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>596037700</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>771229440</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-65A8-4DE3-BF3F-CFB5EB5C0F60}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="53169167"/>
+        <c:axId val="53180687"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="53169167"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="53180687"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="53180687"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="53169167"/>
+        <c:crossesAt val="0"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Gráfico 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B63D5F72-0A81-6D4D-01CE-455D20F5A258}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -190,7 +1095,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -296,7 +1201,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -438,7 +1343,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -446,10 +1351,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0481484C-C14D-48FC-BD21-56BD73C05859}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,26 +1392,26 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>235356</v>
+        <v>324</v>
       </c>
       <c r="B2" s="1">
-        <v>2851799</v>
+        <v>46500</v>
       </c>
       <c r="C2" s="1">
-        <v>2835500</v>
+        <v>54400</v>
       </c>
       <c r="D2" s="1">
-        <v>2823900</v>
+        <v>49400</v>
       </c>
       <c r="E2" s="1">
-        <v>2841300</v>
+        <v>54000</v>
       </c>
       <c r="F2" s="1">
-        <v>2849900</v>
+        <v>45800</v>
       </c>
       <c r="G2" s="1">
         <f>AVERAGE(B2:F2)</f>
-        <v>2840479.8</v>
+        <v>50020</v>
       </c>
       <c r="I2" t="s">
         <v>7</v>
@@ -514,26 +1419,26 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>5235124</v>
+        <v>43423</v>
       </c>
       <c r="B3" s="1">
-        <v>15795300</v>
+        <v>507300</v>
       </c>
       <c r="C3" s="1">
-        <v>16061600</v>
+        <v>600000</v>
       </c>
       <c r="D3" s="1">
-        <v>15428900</v>
+        <v>597800</v>
       </c>
       <c r="E3" s="1">
-        <v>21230800</v>
+        <v>594800</v>
       </c>
       <c r="F3" s="1">
-        <v>15668900</v>
+        <v>596300</v>
       </c>
       <c r="G3" s="1">
-        <f t="shared" ref="G3:G11" si="0">AVERAGE(B3:F3)</f>
-        <v>16837100</v>
+        <f>AVERAGE(B3:F3)</f>
+        <v>579240</v>
       </c>
       <c r="I3" t="s">
         <v>8</v>
@@ -541,26 +1446,26 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>565235323</v>
+        <v>235356</v>
       </c>
       <c r="B4" s="1">
-        <v>1142948900</v>
+        <v>2851799</v>
       </c>
       <c r="C4" s="1">
-        <v>1149516900</v>
+        <v>2835500</v>
       </c>
       <c r="D4" s="1">
-        <v>1144251200</v>
+        <v>2823900</v>
       </c>
       <c r="E4" s="1">
-        <v>1134278500</v>
+        <v>2841300</v>
       </c>
       <c r="F4" s="1">
-        <v>1134145500</v>
+        <v>2849900</v>
       </c>
       <c r="G4" s="1">
-        <f t="shared" si="0"/>
-        <v>1141028200</v>
+        <f>AVERAGE(B4:F4)</f>
+        <v>2840479.8</v>
       </c>
       <c r="I4" t="s">
         <v>13</v>
@@ -568,98 +1473,98 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>21213213</v>
+        <v>234324</v>
       </c>
       <c r="B5" s="1">
-        <v>48818400</v>
+        <v>2848400</v>
       </c>
       <c r="C5" s="1">
-        <v>49095600</v>
+        <v>2831500</v>
       </c>
       <c r="D5" s="1">
-        <v>48813200</v>
+        <v>2971100</v>
       </c>
       <c r="E5" s="1">
-        <v>48461100</v>
+        <v>2885700</v>
       </c>
       <c r="F5" s="1">
-        <v>48751300</v>
+        <v>2900900</v>
       </c>
       <c r="G5" s="1">
-        <f t="shared" si="0"/>
-        <v>48787920</v>
+        <f>AVERAGE(B5:F5)</f>
+        <v>2887520</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>234324</v>
+        <v>5654774</v>
       </c>
       <c r="B6" s="1">
-        <v>2848400</v>
+        <v>16253400</v>
       </c>
       <c r="C6" s="1">
-        <v>2831500</v>
+        <v>16771200</v>
       </c>
       <c r="D6" s="1">
-        <v>2971100</v>
+        <v>16832600</v>
       </c>
       <c r="E6" s="1">
-        <v>2885700</v>
+        <v>16827600</v>
       </c>
       <c r="F6" s="1">
-        <v>2900900</v>
+        <v>16483100</v>
       </c>
       <c r="G6" s="1">
-        <f t="shared" si="0"/>
-        <v>2887520</v>
+        <f>AVERAGE(B6:F6)</f>
+        <v>16633580</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>43423</v>
+        <v>5235124</v>
       </c>
       <c r="B7" s="1">
-        <v>507300</v>
+        <v>15795300</v>
       </c>
       <c r="C7" s="1">
-        <v>600000</v>
+        <v>16061600</v>
       </c>
       <c r="D7" s="1">
-        <v>597800</v>
+        <v>15428900</v>
       </c>
       <c r="E7" s="1">
-        <v>594800</v>
+        <v>21230800</v>
       </c>
       <c r="F7" s="1">
-        <v>596300</v>
+        <v>15668900</v>
       </c>
       <c r="G7" s="1">
-        <f t="shared" si="0"/>
-        <v>579240</v>
+        <f>AVERAGE(B7:F7)</f>
+        <v>16837100</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>5654774</v>
+        <v>21213213</v>
       </c>
       <c r="B8" s="1">
-        <v>16253400</v>
+        <v>48818400</v>
       </c>
       <c r="C8" s="1">
-        <v>16771200</v>
+        <v>49095600</v>
       </c>
       <c r="D8" s="1">
-        <v>16832600</v>
+        <v>48813200</v>
       </c>
       <c r="E8" s="1">
-        <v>16827600</v>
+        <v>48461100</v>
       </c>
       <c r="F8" s="1">
-        <v>16483100</v>
+        <v>48751300</v>
       </c>
       <c r="G8" s="1">
-        <f t="shared" si="0"/>
-        <v>16633580</v>
+        <f>AVERAGE(B8:F8)</f>
+        <v>48787920</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -682,7 +1587,7 @@
         <v>127974900</v>
       </c>
       <c r="G9" s="1">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(B9:F9)</f>
         <v>122103980</v>
       </c>
     </row>
@@ -706,32 +1611,32 @@
         <v>924074100</v>
       </c>
       <c r="G10" s="1">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(B10:F10)</f>
         <v>926483520</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>324</v>
+        <v>565235323</v>
       </c>
       <c r="B11" s="1">
-        <v>46500</v>
+        <v>1142948900</v>
       </c>
       <c r="C11" s="1">
-        <v>54400</v>
+        <v>1149516900</v>
       </c>
       <c r="D11" s="1">
-        <v>49400</v>
+        <v>1144251200</v>
       </c>
       <c r="E11" s="1">
-        <v>54000</v>
+        <v>1134278500</v>
       </c>
       <c r="F11" s="1">
-        <v>45800</v>
+        <v>1134145500</v>
       </c>
       <c r="G11" s="1">
-        <f t="shared" si="0"/>
-        <v>50020</v>
+        <f>AVERAGE(B11:F11)</f>
+        <v>1141028200</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -762,26 +1667,26 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>235356</v>
+        <v>324</v>
       </c>
       <c r="B14" s="1">
-        <v>2034000</v>
+        <v>32500</v>
       </c>
       <c r="C14" s="1">
-        <v>1905500</v>
+        <v>32400</v>
       </c>
       <c r="D14" s="1">
-        <v>1758400</v>
+        <v>32900</v>
       </c>
       <c r="E14" s="1">
-        <v>1682400</v>
+        <v>39700</v>
       </c>
       <c r="F14" s="1">
-        <v>1776500</v>
+        <v>37000</v>
       </c>
       <c r="G14" s="1">
         <f>AVERAGE(B14:F14)</f>
-        <v>1831360</v>
+        <v>34900</v>
       </c>
       <c r="I14" t="s">
         <v>9</v>
@@ -789,26 +1694,26 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>5235124</v>
+        <v>43423</v>
       </c>
       <c r="B15" s="1">
-        <v>24932200</v>
+        <v>658600</v>
       </c>
       <c r="C15" s="1">
-        <v>23580600</v>
+        <v>531400</v>
       </c>
       <c r="D15" s="1">
-        <v>10376500</v>
+        <v>545200</v>
       </c>
       <c r="E15" s="1">
-        <v>10214900</v>
+        <v>633300</v>
       </c>
       <c r="F15" s="1">
-        <v>24835900</v>
+        <v>527600</v>
       </c>
       <c r="G15" s="1">
-        <f t="shared" ref="G15:G23" si="1">AVERAGE(B15:F15)</f>
-        <v>18788020</v>
+        <f>AVERAGE(B15:F15)</f>
+        <v>579220</v>
       </c>
       <c r="I15" t="s">
         <v>10</v>
@@ -816,128 +1721,128 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>565235323</v>
+        <v>234324</v>
       </c>
       <c r="B16" s="1">
-        <v>771694800</v>
+        <v>1677200</v>
       </c>
       <c r="C16" s="1">
-        <v>769228100</v>
+        <v>1711300</v>
       </c>
       <c r="D16" s="1">
-        <v>768799700</v>
+        <v>1878300</v>
       </c>
       <c r="E16" s="1">
-        <v>770057600</v>
+        <v>1759400</v>
       </c>
       <c r="F16" s="1">
-        <v>776367000</v>
+        <v>1826100</v>
       </c>
       <c r="G16" s="1">
-        <f t="shared" si="1"/>
-        <v>771229440</v>
+        <f>AVERAGE(B16:F16)</f>
+        <v>1770460</v>
       </c>
       <c r="I16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
+        <v>235356</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2034000</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1905500</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1758400</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1682400</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1776500</v>
+      </c>
+      <c r="G17" s="1">
+        <f>AVERAGE(B17:F17)</f>
+        <v>1831360</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>5654774</v>
+      </c>
+      <c r="B18" s="1">
+        <v>10763700</v>
+      </c>
+      <c r="C18" s="1">
+        <v>23961400</v>
+      </c>
+      <c r="D18" s="1">
+        <v>24344500</v>
+      </c>
+      <c r="E18" s="1">
+        <v>10761400</v>
+      </c>
+      <c r="F18" s="1">
+        <v>23436800</v>
+      </c>
+      <c r="G18" s="1">
+        <f>AVERAGE(B18:F18)</f>
+        <v>18653560</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>5235124</v>
+      </c>
+      <c r="B19" s="1">
+        <v>24932200</v>
+      </c>
+      <c r="C19" s="1">
+        <v>23580600</v>
+      </c>
+      <c r="D19" s="1">
+        <v>10376500</v>
+      </c>
+      <c r="E19" s="1">
+        <v>10214900</v>
+      </c>
+      <c r="F19" s="1">
+        <v>24835900</v>
+      </c>
+      <c r="G19" s="1">
+        <f>AVERAGE(B19:F19)</f>
+        <v>18788020</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>21213213</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B20" s="1">
         <v>33159500</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C20" s="1">
         <v>31755400</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D20" s="1">
         <v>34621100</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E20" s="1">
         <v>33740800</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F20" s="1">
         <v>32059900</v>
       </c>
-      <c r="G17" s="1">
-        <f t="shared" si="1"/>
+      <c r="G20" s="1">
+        <f>AVERAGE(B20:F20)</f>
         <v>33067340</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>234324</v>
-      </c>
-      <c r="B18" s="1">
-        <v>1677200</v>
-      </c>
-      <c r="C18" s="1">
-        <v>1711300</v>
-      </c>
-      <c r="D18" s="1">
-        <v>1878300</v>
-      </c>
-      <c r="E18" s="1">
-        <v>1759400</v>
-      </c>
-      <c r="F18" s="1">
-        <v>1826100</v>
-      </c>
-      <c r="G18" s="1">
-        <f t="shared" si="1"/>
-        <v>1770460</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>43423</v>
-      </c>
-      <c r="B19" s="1">
-        <v>658600</v>
-      </c>
-      <c r="C19" s="1">
-        <v>531400</v>
-      </c>
-      <c r="D19" s="1">
-        <v>545200</v>
-      </c>
-      <c r="E19" s="1">
-        <v>633300</v>
-      </c>
-      <c r="F19" s="1">
-        <v>527600</v>
-      </c>
-      <c r="G19" s="1">
-        <f t="shared" si="1"/>
-        <v>579220</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>5654774</v>
-      </c>
-      <c r="B20" s="1">
-        <v>10763700</v>
-      </c>
-      <c r="C20" s="1">
-        <v>23961400</v>
-      </c>
-      <c r="D20" s="1">
-        <v>24344500</v>
-      </c>
-      <c r="E20" s="1">
-        <v>10761400</v>
-      </c>
-      <c r="F20" s="1">
-        <v>23436800</v>
-      </c>
-      <c r="G20" s="1">
-        <f t="shared" si="1"/>
-        <v>18653560</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>56863435</v>
       </c>
@@ -957,11 +1862,14 @@
         <v>80427800</v>
       </c>
       <c r="G21" s="1">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(B21:F21)</f>
         <v>80661940</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>436346436</v>
       </c>
@@ -981,38 +1889,44 @@
         <v>595088200</v>
       </c>
       <c r="G22" s="1">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(B22:F22)</f>
         <v>596037700</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>324</v>
+        <v>565235323</v>
       </c>
       <c r="B23" s="1">
-        <v>32500</v>
+        <v>771694800</v>
       </c>
       <c r="C23" s="1">
-        <v>32400</v>
+        <v>769228100</v>
       </c>
       <c r="D23" s="1">
-        <v>32900</v>
+        <v>768799700</v>
       </c>
       <c r="E23" s="1">
-        <v>39700</v>
+        <v>770057600</v>
       </c>
       <c r="F23" s="1">
-        <v>37000</v>
+        <v>776367000</v>
       </c>
       <c r="G23" s="1">
-        <f t="shared" si="1"/>
-        <v>34900</v>
+        <f>AVERAGE(B23:F23)</f>
+        <v>771229440</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I25" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A14:G23">
+    <sortCondition ref="G14:G23"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="G2:G11" formulaRange="1"/>
-  </ignoredErrors>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se agregaron 2 tablas en el excel
</commit_message>
<xml_diff>
--- a/numero_perfecto/pruebas.xlsx
+++ b/numero_perfecto/pruebas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC28\Documents\Analisis-Algoritmos\numero_perfecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EDA5189-5A01-4FA3-8B15-D260C937EE27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310EE1EC-C92D-48EB-A3E0-4F4FA7B84AD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{119C92B1-EED5-41A3-9A3B-CFA0F4C48975}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{119C92B1-EED5-41A3-9A3B-CFA0F4C48975}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="18">
   <si>
     <t>T1</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t xml:space="preserve">     </t>
+  </si>
+  <si>
+    <t>Codigo compañero</t>
   </si>
 </sst>
 </file>
@@ -1351,10 +1354,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0481484C-C14D-48FC-BD21-56BD73C05859}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1410,7 +1413,7 @@
         <v>45800</v>
       </c>
       <c r="G2" s="1">
-        <f>AVERAGE(B2:F2)</f>
+        <f t="shared" ref="G2:G11" si="0">AVERAGE(B2:F2)</f>
         <v>50020</v>
       </c>
       <c r="I2" t="s">
@@ -1437,7 +1440,7 @@
         <v>596300</v>
       </c>
       <c r="G3" s="1">
-        <f>AVERAGE(B3:F3)</f>
+        <f t="shared" si="0"/>
         <v>579240</v>
       </c>
       <c r="I3" t="s">
@@ -1464,7 +1467,7 @@
         <v>2849900</v>
       </c>
       <c r="G4" s="1">
-        <f>AVERAGE(B4:F4)</f>
+        <f t="shared" si="0"/>
         <v>2840479.8</v>
       </c>
       <c r="I4" t="s">
@@ -1491,7 +1494,7 @@
         <v>2900900</v>
       </c>
       <c r="G5" s="1">
-        <f>AVERAGE(B5:F5)</f>
+        <f t="shared" si="0"/>
         <v>2887520</v>
       </c>
     </row>
@@ -1515,7 +1518,7 @@
         <v>16483100</v>
       </c>
       <c r="G6" s="1">
-        <f>AVERAGE(B6:F6)</f>
+        <f t="shared" si="0"/>
         <v>16633580</v>
       </c>
     </row>
@@ -1539,7 +1542,7 @@
         <v>15668900</v>
       </c>
       <c r="G7" s="1">
-        <f>AVERAGE(B7:F7)</f>
+        <f t="shared" si="0"/>
         <v>16837100</v>
       </c>
     </row>
@@ -1563,7 +1566,7 @@
         <v>48751300</v>
       </c>
       <c r="G8" s="1">
-        <f>AVERAGE(B8:F8)</f>
+        <f t="shared" si="0"/>
         <v>48787920</v>
       </c>
     </row>
@@ -1587,7 +1590,7 @@
         <v>127974900</v>
       </c>
       <c r="G9" s="1">
-        <f>AVERAGE(B9:F9)</f>
+        <f t="shared" si="0"/>
         <v>122103980</v>
       </c>
     </row>
@@ -1611,7 +1614,7 @@
         <v>924074100</v>
       </c>
       <c r="G10" s="1">
-        <f>AVERAGE(B10:F10)</f>
+        <f t="shared" si="0"/>
         <v>926483520</v>
       </c>
     </row>
@@ -1635,7 +1638,7 @@
         <v>1134145500</v>
       </c>
       <c r="G11" s="1">
-        <f>AVERAGE(B11:F11)</f>
+        <f t="shared" si="0"/>
         <v>1141028200</v>
       </c>
     </row>
@@ -1685,7 +1688,7 @@
         <v>37000</v>
       </c>
       <c r="G14" s="1">
-        <f>AVERAGE(B14:F14)</f>
+        <f t="shared" ref="G14:G23" si="1">AVERAGE(B14:F14)</f>
         <v>34900</v>
       </c>
       <c r="I14" t="s">
@@ -1712,7 +1715,7 @@
         <v>527600</v>
       </c>
       <c r="G15" s="1">
-        <f>AVERAGE(B15:F15)</f>
+        <f t="shared" si="1"/>
         <v>579220</v>
       </c>
       <c r="I15" t="s">
@@ -1739,7 +1742,7 @@
         <v>1826100</v>
       </c>
       <c r="G16" s="1">
-        <f>AVERAGE(B16:F16)</f>
+        <f t="shared" si="1"/>
         <v>1770460</v>
       </c>
       <c r="I16" t="s">
@@ -1766,7 +1769,7 @@
         <v>1776500</v>
       </c>
       <c r="G17" s="1">
-        <f>AVERAGE(B17:F17)</f>
+        <f t="shared" si="1"/>
         <v>1831360</v>
       </c>
     </row>
@@ -1790,7 +1793,7 @@
         <v>23436800</v>
       </c>
       <c r="G18" s="1">
-        <f>AVERAGE(B18:F18)</f>
+        <f t="shared" si="1"/>
         <v>18653560</v>
       </c>
     </row>
@@ -1814,7 +1817,7 @@
         <v>24835900</v>
       </c>
       <c r="G19" s="1">
-        <f>AVERAGE(B19:F19)</f>
+        <f t="shared" si="1"/>
         <v>18788020</v>
       </c>
     </row>
@@ -1838,7 +1841,7 @@
         <v>32059900</v>
       </c>
       <c r="G20" s="1">
-        <f>AVERAGE(B20:F20)</f>
+        <f t="shared" si="1"/>
         <v>33067340</v>
       </c>
     </row>
@@ -1862,7 +1865,7 @@
         <v>80427800</v>
       </c>
       <c r="G21" s="1">
-        <f>AVERAGE(B21:F21)</f>
+        <f t="shared" si="1"/>
         <v>80661940</v>
       </c>
       <c r="I21" t="s">
@@ -1889,7 +1892,7 @@
         <v>595088200</v>
       </c>
       <c r="G22" s="1">
-        <f>AVERAGE(B22:F22)</f>
+        <f t="shared" si="1"/>
         <v>596037700</v>
       </c>
     </row>
@@ -1913,13 +1916,571 @@
         <v>776367000</v>
       </c>
       <c r="G23" s="1">
-        <f>AVERAGE(B23:F23)</f>
+        <f t="shared" si="1"/>
         <v>771229440</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>17</v>
+      </c>
       <c r="I25" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26" t="s">
+        <v>3</v>
+      </c>
+      <c r="F26" t="s">
+        <v>4</v>
+      </c>
+      <c r="G26" t="s">
+        <v>6</v>
+      </c>
+      <c r="I26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>324</v>
+      </c>
+      <c r="B27" s="1">
+        <v>106900</v>
+      </c>
+      <c r="C27" s="1">
+        <v>107500</v>
+      </c>
+      <c r="D27" s="1">
+        <v>107500</v>
+      </c>
+      <c r="E27" s="1">
+        <v>106400</v>
+      </c>
+      <c r="F27" s="1">
+        <v>171400</v>
+      </c>
+      <c r="G27" s="1">
+        <f t="shared" ref="G27:G36" si="2">AVERAGE(B27:F27)</f>
+        <v>119940</v>
+      </c>
+      <c r="I27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>43423</v>
+      </c>
+      <c r="B28" s="1">
+        <v>495300</v>
+      </c>
+      <c r="C28" s="1">
+        <v>495000</v>
+      </c>
+      <c r="D28" s="1">
+        <v>432400</v>
+      </c>
+      <c r="E28" s="1">
+        <v>498100</v>
+      </c>
+      <c r="F28" s="1">
+        <v>503200</v>
+      </c>
+      <c r="G28" s="1">
+        <f t="shared" si="2"/>
+        <v>484800</v>
+      </c>
+      <c r="I28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>235356</v>
+      </c>
+      <c r="B29" s="1">
+        <v>2211500</v>
+      </c>
+      <c r="C29" s="1">
+        <v>2209000</v>
+      </c>
+      <c r="D29" s="1">
+        <v>2206900</v>
+      </c>
+      <c r="E29" s="1">
+        <v>2228100</v>
+      </c>
+      <c r="F29" s="1">
+        <v>2209700</v>
+      </c>
+      <c r="G29" s="1">
+        <f t="shared" si="2"/>
+        <v>2213040</v>
+      </c>
+      <c r="I29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>234324</v>
+      </c>
+      <c r="B30" s="1">
+        <v>2206500</v>
+      </c>
+      <c r="C30" s="1">
+        <v>2203500</v>
+      </c>
+      <c r="D30" s="1">
+        <v>1576600</v>
+      </c>
+      <c r="E30" s="1">
+        <v>2231300</v>
+      </c>
+      <c r="F30" s="1">
+        <v>2205000</v>
+      </c>
+      <c r="G30" s="1">
+        <f t="shared" si="2"/>
+        <v>2084580</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>5654774</v>
+      </c>
+      <c r="B31" s="1">
+        <v>10027600</v>
+      </c>
+      <c r="C31" s="1">
+        <v>8015100</v>
+      </c>
+      <c r="D31" s="1">
+        <v>9489800</v>
+      </c>
+      <c r="E31" s="1">
+        <v>12047400</v>
+      </c>
+      <c r="F31" s="1">
+        <v>9545200</v>
+      </c>
+      <c r="G31" s="1">
+        <f t="shared" si="2"/>
+        <v>9825020</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>5235124</v>
+      </c>
+      <c r="B32" s="1">
+        <v>10734400</v>
+      </c>
+      <c r="C32" s="1">
+        <v>11586500</v>
+      </c>
+      <c r="D32" s="1">
+        <v>10644100</v>
+      </c>
+      <c r="E32" s="1">
+        <v>12594400</v>
+      </c>
+      <c r="F32" s="1">
+        <v>14598100</v>
+      </c>
+      <c r="G32" s="1">
+        <f t="shared" si="2"/>
+        <v>12031500</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>21213213</v>
+      </c>
+      <c r="B33" s="1">
+        <v>26071500</v>
+      </c>
+      <c r="C33" s="1">
+        <v>27385000</v>
+      </c>
+      <c r="D33" s="1">
+        <v>26859500</v>
+      </c>
+      <c r="E33" s="1">
+        <v>25500600</v>
+      </c>
+      <c r="F33" s="1">
+        <v>26957400</v>
+      </c>
+      <c r="G33" s="1">
+        <f t="shared" si="2"/>
+        <v>26554800</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>56863435</v>
+      </c>
+      <c r="B34" s="1">
+        <v>62803800</v>
+      </c>
+      <c r="C34" s="1">
+        <v>62790100</v>
+      </c>
+      <c r="D34" s="1">
+        <v>64514800</v>
+      </c>
+      <c r="E34" s="1">
+        <v>61111600</v>
+      </c>
+      <c r="F34" s="1">
+        <v>71477400</v>
+      </c>
+      <c r="G34" s="1">
+        <f t="shared" si="2"/>
+        <v>64539540</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>436346436</v>
+      </c>
+      <c r="B35" s="1">
+        <v>444088700</v>
+      </c>
+      <c r="C35" s="1">
+        <v>439661300</v>
+      </c>
+      <c r="D35" s="1">
+        <v>436972400</v>
+      </c>
+      <c r="E35" s="1">
+        <v>446940100</v>
+      </c>
+      <c r="F35" s="1">
+        <v>438637300</v>
+      </c>
+      <c r="G35" s="1">
+        <f t="shared" si="2"/>
+        <v>441259960</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>565235323</v>
+      </c>
+      <c r="B36" s="1">
+        <v>543234200</v>
+      </c>
+      <c r="C36" s="1">
+        <v>543758000</v>
+      </c>
+      <c r="D36" s="1">
+        <v>549920600</v>
+      </c>
+      <c r="E36" s="1">
+        <v>557457400</v>
+      </c>
+      <c r="F36" s="1">
+        <v>542130600</v>
+      </c>
+      <c r="G36" s="1">
+        <f t="shared" si="2"/>
+        <v>547300160</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39" t="s">
+        <v>2</v>
+      </c>
+      <c r="E39" t="s">
+        <v>3</v>
+      </c>
+      <c r="F39" t="s">
+        <v>4</v>
+      </c>
+      <c r="G39" t="s">
+        <v>6</v>
+      </c>
+      <c r="I39" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>324</v>
+      </c>
+      <c r="B40" s="1">
+        <v>113800</v>
+      </c>
+      <c r="C40" s="1">
+        <v>107800</v>
+      </c>
+      <c r="D40" s="1">
+        <v>107200</v>
+      </c>
+      <c r="E40" s="1">
+        <v>107200</v>
+      </c>
+      <c r="F40" s="1">
+        <v>107900</v>
+      </c>
+      <c r="G40" s="1">
+        <f t="shared" ref="G40:G49" si="3">AVERAGE(B40:F40)</f>
+        <v>108780</v>
+      </c>
+      <c r="I40" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>43423</v>
+      </c>
+      <c r="B41" s="1">
+        <v>350000</v>
+      </c>
+      <c r="C41" s="1">
+        <v>496300</v>
+      </c>
+      <c r="D41" s="1">
+        <v>490700</v>
+      </c>
+      <c r="E41" s="1">
+        <v>349800</v>
+      </c>
+      <c r="F41" s="1">
+        <v>495800</v>
+      </c>
+      <c r="G41" s="1">
+        <f t="shared" si="3"/>
+        <v>436520</v>
+      </c>
+      <c r="I41" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>235356</v>
+      </c>
+      <c r="B42" s="1">
+        <v>2213100</v>
+      </c>
+      <c r="C42" s="1">
+        <v>2213600</v>
+      </c>
+      <c r="D42" s="1">
+        <v>2209600</v>
+      </c>
+      <c r="E42" s="1">
+        <v>2070300</v>
+      </c>
+      <c r="F42" s="1">
+        <v>2217500</v>
+      </c>
+      <c r="G42" s="1">
+        <f t="shared" si="3"/>
+        <v>2184820</v>
+      </c>
+      <c r="I42" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>234324</v>
+      </c>
+      <c r="B43" s="1">
+        <v>2206800</v>
+      </c>
+      <c r="C43" s="1">
+        <v>1529200</v>
+      </c>
+      <c r="D43" s="1">
+        <v>2205000</v>
+      </c>
+      <c r="E43" s="1">
+        <v>2204600</v>
+      </c>
+      <c r="F43" s="1">
+        <v>2188100</v>
+      </c>
+      <c r="G43" s="1">
+        <f t="shared" si="3"/>
+        <v>2066740</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>5654774</v>
+      </c>
+      <c r="B44" s="1">
+        <v>9557400</v>
+      </c>
+      <c r="C44" s="1">
+        <v>9632500</v>
+      </c>
+      <c r="D44" s="1">
+        <v>9471600</v>
+      </c>
+      <c r="E44" s="1">
+        <v>8026900</v>
+      </c>
+      <c r="F44" s="1">
+        <v>9587900</v>
+      </c>
+      <c r="G44" s="1">
+        <f t="shared" si="3"/>
+        <v>9255260</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>5235124</v>
+      </c>
+      <c r="B45" s="1">
+        <v>9218700</v>
+      </c>
+      <c r="C45" s="1">
+        <v>10774500</v>
+      </c>
+      <c r="D45" s="1">
+        <v>9158700</v>
+      </c>
+      <c r="E45" s="1">
+        <v>10814800</v>
+      </c>
+      <c r="F45" s="1">
+        <v>11239400</v>
+      </c>
+      <c r="G45" s="1">
+        <f t="shared" si="3"/>
+        <v>10241220</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>21213213</v>
+      </c>
+      <c r="B46" s="1">
+        <v>33986600</v>
+      </c>
+      <c r="C46" s="1">
+        <v>31427400</v>
+      </c>
+      <c r="D46" s="1">
+        <v>27271300</v>
+      </c>
+      <c r="E46" s="1">
+        <v>25931500</v>
+      </c>
+      <c r="F46" s="1">
+        <v>26964400</v>
+      </c>
+      <c r="G46" s="1">
+        <f t="shared" si="3"/>
+        <v>29116240</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>56863435</v>
+      </c>
+      <c r="B47" s="1">
+        <v>79262600</v>
+      </c>
+      <c r="C47" s="1">
+        <v>69104400</v>
+      </c>
+      <c r="D47" s="1">
+        <v>69605200</v>
+      </c>
+      <c r="E47" s="1">
+        <v>61927400</v>
+      </c>
+      <c r="F47" s="1">
+        <v>65044800</v>
+      </c>
+      <c r="G47" s="1">
+        <f t="shared" si="3"/>
+        <v>68988880</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>436346436</v>
+      </c>
+      <c r="B48" s="1">
+        <v>442941900</v>
+      </c>
+      <c r="C48" s="1">
+        <v>445144600</v>
+      </c>
+      <c r="D48" s="1">
+        <v>439727300</v>
+      </c>
+      <c r="E48" s="1">
+        <v>442382500</v>
+      </c>
+      <c r="F48" s="1">
+        <v>439424200</v>
+      </c>
+      <c r="G48" s="1">
+        <f t="shared" si="3"/>
+        <v>441924100</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>565235323</v>
+      </c>
+      <c r="B49" s="1">
+        <v>553828300</v>
+      </c>
+      <c r="C49" s="1">
+        <v>544060500</v>
+      </c>
+      <c r="D49" s="1">
+        <v>551903100</v>
+      </c>
+      <c r="E49" s="1">
+        <v>542087000</v>
+      </c>
+      <c r="F49" s="1">
+        <v>549775400</v>
+      </c>
+      <c r="G49" s="1">
+        <f t="shared" si="3"/>
+        <v>548330860</v>
       </c>
     </row>
   </sheetData>

</xml_diff>